<commit_message>
more pandera amendments and new feedstock prices sheet
</commit_message>
<xml_diff>
--- a/mppsteel/data/import_data/Feedstock Prices.xlsx
+++ b/mppsteel/data/import_data/Feedstock Prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{8A860862-830F-487D-AF1E-50CDDEEF4A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E4918A6-F5B0-45F7-B20A-C1DE8069A7F1}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{8A860862-830F-487D-AF1E-50CDDEEF4A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5740AF2D-95A9-4C32-8A8E-DB0DFED03807}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" xr2:uid="{28E9977C-84A3-43AD-AF96-4E089B66DB2E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19433" windowHeight="13187" xr2:uid="{28E9977C-84A3-43AD-AF96-4E089B66DB2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Year</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Excel Tab</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
   </si>
   <si>
     <t>Other slag</t>
-  </si>
-  <si>
-    <t>Price &amp; Emission parameters</t>
   </si>
   <si>
     <t>Unit</t>
@@ -490,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD737EBA-DB48-47D6-90C0-A418E594C1DA}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -513,40 +507,35 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>2020</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
       <c r="D2">
         <f>97.73*0.877</f>
         <v>85.709209999999999</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
@@ -554,23 +543,20 @@
         <v>2020</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <f>224.46*0.877</f>
         <v>196.85142000000002</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
@@ -578,23 +564,20 @@
         <v>2020</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <f>300.67*0.877</f>
         <v>263.68759</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
@@ -602,23 +585,20 @@
         <v>2020</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3">
         <f>121.86*0.877</f>
         <v>106.87121999999999</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
@@ -626,23 +606,20 @@
         <v>2020</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <f>-27.5*0.877/1000</f>
         <v>-2.41175E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
@@ -650,22 +627,19 @@
         <v>2020</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
@@ -686,14 +660,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f94796c5baa2ef88ac6145701948dc8f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e880ceb9264c792c54763cc60e020778" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cc653c178d9ffcb24786b6a9d53371f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3af53c5407280ad7b07c166bc7f6511a" ns2:_="" ns3:_="">
     <xsd:import namespace="b44fa922-a688-4301-8945-67f7597c9c55"/>
     <xsd:import namespace="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
     <xsd:element name="properties">
@@ -706,6 +683,14 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -724,6 +709,50 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -857,33 +886,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44FEDDF4-819D-45CF-9D9D-71A79C44C95F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA233994-C021-4EE2-891B-792745C54C2D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b44fa922-a688-4301-8945-67f7597c9c55"/>
-    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65125D1D-26F7-4563-82CF-385ED34B3F9C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EA15C06-6D72-4BAD-9DCE-41F94F58EC54}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -902,9 +919,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA233994-C021-4EE2-891B-792745C54C2D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44FEDDF4-819D-45CF-9D9D-71A79C44C95F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="b44fa922-a688-4301-8945-67f7597c9c55"/>
+    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>